<commit_message>
sydw===jj Signed-off-by: fengjinliang <475185283@qq.com>
</commit_message>
<xml_diff>
--- a/sydw/2020上/考点/考点.xlsx
+++ b/sydw/2020上/考点/考点.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="11820" windowHeight="12150" activeTab="5"/>
+    <workbookView windowWidth="19200" windowHeight="7140"/>
   </bookViews>
   <sheets>
     <sheet name="题型" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="223">
   <si>
     <t>判断题</t>
   </si>
@@ -43,6 +43,24 @@
   </si>
   <si>
     <t>案例分析</t>
+  </si>
+  <si>
+    <t>制度</t>
+  </si>
+  <si>
+    <t>是政治词汇</t>
+  </si>
+  <si>
+    <t>经济制度</t>
+  </si>
+  <si>
+    <t>体制</t>
+  </si>
+  <si>
+    <t>是行业词汇</t>
+  </si>
+  <si>
+    <t>经济体制</t>
   </si>
   <si>
     <t>2019新增法律法规</t>
@@ -701,6 +719,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <i/>
+        <sz val="11.3"/>
+        <color rgb="FF629755"/>
+        <rFont val="Fira Code"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">* </t>
     </r>
     <r>
@@ -716,6 +741,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <i/>
+        <sz val="11.3"/>
+        <color rgb="FF629755"/>
+        <rFont val="Fira Code"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">* </t>
     </r>
     <r>
@@ -735,10 +767,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -790,16 +822,32 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -810,9 +858,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -826,9 +881,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -844,25 +914,17 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -875,7 +937,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -890,37 +952,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -959,66 +991,162 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1031,109 +1159,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1147,13 +1179,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1173,21 +1209,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1199,15 +1220,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1229,9 +1241,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1244,6 +1258,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1252,10 +1284,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1267,16 +1299,16 @@
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1285,112 +1317,112 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1779,13 +1811,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="C3:M11"/>
+  <dimension ref="C3:M17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <sheetData>
     <row r="3" spans="3:3">
       <c r="C3" t="s">
@@ -1821,6 +1853,28 @@
     <row r="11" spans="3:3">
       <c r="C11" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="5:8">
+      <c r="E16" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="5:8">
+      <c r="E17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" t="s">
+        <v>12</v>
+      </c>
+      <c r="H17" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1839,40 +1893,40 @@
       <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="5"/>
   <cols>
-    <col min="3" max="3" width="17.7583333333333" customWidth="1"/>
-    <col min="4" max="4" width="36.5416666666667" customWidth="1"/>
-    <col min="6" max="6" width="11.8166666666667" style="7"/>
+    <col min="3" max="3" width="17.7545454545455" customWidth="1"/>
+    <col min="4" max="4" width="36.5454545454545" customWidth="1"/>
+    <col min="6" max="6" width="11.8181818181818" style="7"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:4">
       <c r="C2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="5:6">
       <c r="E5" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="4:6">
       <c r="D6" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="4:6">
       <c r="D7" s="10" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F7" s="11">
         <v>43739</v>
@@ -1880,22 +1934,22 @@
     </row>
     <row r="13" spans="4:4">
       <c r="D13" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="4:4">
       <c r="D14" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="4:4">
       <c r="D15" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="4:4">
       <c r="D16" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1917,83 +1971,83 @@
       <selection activeCell="M16" sqref="M16:M23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
     <col min="3" max="3" width="9" style="7"/>
   </cols>
   <sheetData>
     <row r="1" ht="25.5" spans="5:5">
       <c r="E1" s="8" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" ht="25.5" spans="5:5">
       <c r="E2" s="8" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" ht="25.5" spans="5:5">
       <c r="E3" s="8" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" ht="25.5" spans="5:5">
       <c r="E4" s="8" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="6:8">
       <c r="F6" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="H6" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="6:13">
       <c r="F8" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="J8" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="M8" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="10:13">
       <c r="J9" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="L9" s="3"/>
       <c r="M9" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="10:13">
       <c r="J10" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="L10" s="3"/>
       <c r="M10" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="10:13">
       <c r="J11" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="L11" s="3"/>
       <c r="M11" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="2:3">
       <c r="B12" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C12" s="7">
         <v>1980.5</v>
@@ -2001,132 +2055,132 @@
     </row>
     <row r="13" spans="2:6">
       <c r="B13" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="F13" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="2:8">
       <c r="B15" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="F15" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="H15" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="2:13">
       <c r="B16" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C16" s="7">
         <v>1988.4</v>
       </c>
       <c r="M16" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="2:13">
       <c r="B17" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="C17" s="7">
         <v>2010.5</v>
       </c>
       <c r="G17" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="H17" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="M17" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="2:13">
       <c r="B18" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="G18" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="H18" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="M18" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="6:13">
       <c r="F19" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="G19" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="M19" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="7:7">
       <c r="G20" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="7:13">
       <c r="G21" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="M21" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="13:13">
       <c r="M22" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="7:8">
       <c r="G23" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="H23" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="7:8">
       <c r="G24" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="H24" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
     </row>
     <row r="28" spans="7:7">
       <c r="G28" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="29" spans="6:9">
       <c r="F29" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="G29" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="I29" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -2150,138 +2204,138 @@
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.725" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14"/>
   <sheetData>
     <row r="1" spans="4:6">
       <c r="D1" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="F1" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="3:12">
       <c r="C2" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="L2" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="4:12">
       <c r="D3" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="F3" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="L3" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="6:12">
       <c r="F4" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="G4" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="L4" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="7:7">
       <c r="G5" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="6:12">
       <c r="F6" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="L6" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="6:6">
       <c r="F7" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="6:7">
       <c r="F8" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="G8" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="6:12">
       <c r="F10" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="L10" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="4:12">
       <c r="D11" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="F11" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="L11" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="6:12">
       <c r="F12" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="L12" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="6:6">
       <c r="F13" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="6:6">
       <c r="F15" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="6:6">
       <c r="F16" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="6:6">
       <c r="F17" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="3:6">
       <c r="C18" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="F18" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
     </row>
     <row r="19" spans="6:6">
       <c r="F19" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="6:7">
       <c r="F21" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="G21" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -2299,7 +2353,7 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.725" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -2311,252 +2365,252 @@
   <sheetPr/>
   <dimension ref="E1:J88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="5" max="5" width="11.375" customWidth="1"/>
+    <col min="5" max="5" width="11.3727272727273" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="7:10">
       <c r="G1" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="H1" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="I1" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="J1" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="7:10">
       <c r="G2" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="H2" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="I2" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="J2" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="7:10">
       <c r="G3" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="H3" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="I3" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="J3" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="7:10">
       <c r="G4" t="s">
+        <v>114</v>
+      </c>
+      <c r="H4" t="s">
+        <v>115</v>
+      </c>
+      <c r="I4" t="s">
         <v>108</v>
       </c>
-      <c r="H4" t="s">
-        <v>109</v>
-      </c>
-      <c r="I4" t="s">
-        <v>102</v>
-      </c>
       <c r="J4" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="6:7">
       <c r="F7" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="G7" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="6:6">
       <c r="F9" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="6:7">
       <c r="F10" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="G10" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="7:7">
       <c r="G11" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12" spans="5:7">
       <c r="E12" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="F12" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="G12" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
     </row>
     <row r="13" s="1" customFormat="1"/>
     <row r="14" spans="5:7">
       <c r="E14" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="F14" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="G14" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
     </row>
     <row r="15" spans="6:8">
       <c r="F15" s="3" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="G15" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="H15" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" customFormat="1" spans="6:8">
       <c r="F16" s="3"/>
       <c r="G16" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="H16" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
     </row>
     <row r="17" customFormat="1" spans="6:8">
       <c r="F17" s="3"/>
       <c r="G17" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="H17" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
     </row>
     <row r="18" customFormat="1" spans="6:8">
       <c r="F18" s="3"/>
       <c r="G18" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="H18" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
     </row>
     <row r="19" customFormat="1" spans="6:8">
       <c r="F19" s="3"/>
       <c r="G19" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="H19" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
     </row>
     <row r="20" customFormat="1"/>
     <row r="21" s="1" customFormat="1"/>
     <row r="22" spans="7:8">
       <c r="G22" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="H22" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
     </row>
     <row r="23" spans="7:8">
       <c r="G23" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="H23" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
     </row>
     <row r="24" spans="6:8">
       <c r="F24" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="G24" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="H24" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
     </row>
     <row r="25" spans="5:8">
       <c r="E25" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="G25" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="H25" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
     </row>
     <row r="28" spans="6:8">
       <c r="F28" s="4" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="G28" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="H28" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
     </row>
     <row r="29" spans="6:8">
       <c r="F29" s="4"/>
       <c r="G29" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="H29" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
     </row>
     <row r="30" spans="6:6">
       <c r="F30" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
     </row>
     <row r="31" customFormat="1"/>
     <row r="32" customFormat="1" spans="7:8">
       <c r="G32" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="H32" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
     </row>
     <row r="33" customFormat="1" spans="6:6">
       <c r="F33" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
     </row>
     <row r="34" customFormat="1" spans="7:8">
       <c r="G34" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="H34" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
     </row>
     <row r="35" customFormat="1"/>
@@ -2564,40 +2618,40 @@
     <row r="37" s="1" customFormat="1"/>
     <row r="38" spans="7:8">
       <c r="G38" s="3" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="H38" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
     </row>
     <row r="39" spans="7:8">
       <c r="G39" s="3"/>
       <c r="H39" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
     </row>
     <row r="40" spans="6:8">
       <c r="F40" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="G40" s="3"/>
       <c r="H40" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
     <row r="41" spans="7:8">
       <c r="G41" s="3"/>
       <c r="H41" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
     </row>
     <row r="42" spans="5:8">
       <c r="E42" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="G42" s="3"/>
       <c r="H42" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
     </row>
     <row r="43" customFormat="1" spans="7:7">
@@ -2608,7 +2662,7 @@
     </row>
     <row r="45" customFormat="1" spans="6:7">
       <c r="F45" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="G45" s="3"/>
     </row>
@@ -2621,133 +2675,133 @@
     <row r="48" s="1" customFormat="1"/>
     <row r="49" spans="6:7">
       <c r="F49" s="3" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="G49" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
     </row>
     <row r="50" spans="6:7">
       <c r="F50" s="3"/>
       <c r="G50" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
     </row>
     <row r="51" spans="5:7">
       <c r="E51" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="F51" s="3"/>
       <c r="G51" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
     </row>
     <row r="52" spans="6:7">
       <c r="F52" s="3"/>
       <c r="G52" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
     </row>
     <row r="54" spans="6:8">
       <c r="F54" s="3" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="G54" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="H54" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
     </row>
     <row r="55" spans="6:8">
       <c r="F55" s="3"/>
       <c r="G55" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="H55" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
     </row>
     <row r="56" spans="6:8">
       <c r="F56" s="3"/>
       <c r="G56" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="H56" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
     </row>
     <row r="57" spans="6:8">
       <c r="F57" s="3"/>
       <c r="G57" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="H57" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
     </row>
     <row r="58" s="1" customFormat="1"/>
     <row r="59" spans="7:10">
       <c r="G59" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="H59" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="J59" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
     </row>
     <row r="60" spans="7:10">
       <c r="G60" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="I60" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="J60" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
     </row>
     <row r="61" spans="6:10">
       <c r="F61" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="G61" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="J61" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
     </row>
     <row r="62" spans="7:10">
       <c r="G62" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="H62" s="3" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="I62" s="3"/>
       <c r="J62" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
     </row>
     <row r="63" spans="5:10">
       <c r="E63" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="G63" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="H63" s="3"/>
       <c r="I63" s="3"/>
       <c r="J63" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
     </row>
     <row r="64" spans="7:9">
       <c r="G64" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="H64" s="3"/>
       <c r="I64" s="3"/>
@@ -2755,93 +2809,93 @@
     <row r="65" s="1" customFormat="1"/>
     <row r="66" spans="7:9">
       <c r="G66" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="H66" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="I66" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
     </row>
     <row r="67" spans="6:9">
       <c r="F67" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="G67" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="H67" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="I67" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
     </row>
     <row r="68" spans="7:9">
       <c r="G68" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="H68" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="I68" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
     </row>
     <row r="69" spans="7:9">
       <c r="G69" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="H69" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="I69" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
     </row>
     <row r="72" spans="6:7">
       <c r="F72" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="G72" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
     </row>
     <row r="73" spans="7:7">
       <c r="G73" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
     </row>
     <row r="74" spans="7:7">
       <c r="G74" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
     </row>
     <row r="75" spans="7:7">
       <c r="G75" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
     </row>
     <row r="78" s="2" customFormat="1"/>
     <row r="80" spans="6:6">
       <c r="F80" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="86" ht="14.25" spans="7:7">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="86" ht="14.5" spans="7:7">
       <c r="G86" s="5" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="87" ht="14.25" spans="7:7">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="87" ht="14.5" spans="7:7">
       <c r="G87" s="6" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="88" ht="14.25" spans="7:7">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="88" ht="14.5" spans="7:7">
       <c r="G88" s="6" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>